<commit_message>
add time spent in CR2 report
</commit_message>
<xml_diff>
--- a/jEdit_Report_CR2.xlsx
+++ b/jEdit_Report_CR2.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niranjan\Documents\EMSE - Software Maintenance\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="996" yWindow="456" windowWidth="19200" windowHeight="18240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t>Software system:</t>
   </si>
@@ -47,22 +42,7 @@
     <t>Impact analysis</t>
   </si>
   <si>
-    <t>A mins</t>
-  </si>
-  <si>
     <t>Actualization</t>
-  </si>
-  <si>
-    <t>T mins</t>
-  </si>
-  <si>
-    <t>I mins</t>
-  </si>
-  <si>
-    <t>C mins</t>
-  </si>
-  <si>
-    <t>IA mins</t>
   </si>
   <si>
     <t>Testing</t>
@@ -159,6 +139,18 @@
   </si>
   <si>
     <t>All tests passed.</t>
+  </si>
+  <si>
+    <t>30 min</t>
+  </si>
+  <si>
+    <t>480 min</t>
+  </si>
+  <si>
+    <t>60 min</t>
+  </si>
+  <si>
+    <t>660 mins</t>
   </si>
 </sst>
 </file>
@@ -303,7 +295,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -338,7 +330,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -515,7 +507,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -525,260 +517,265 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="66.59765625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="92.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.69921875" style="2"/>
+    <col min="1" max="1" width="66.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="92.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.5">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.5">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.5">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.5">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.5">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15.5">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.5">
       <c r="A7" s="6"/>
       <c r="B7" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.5">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.5">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.5">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="15.5">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="B16" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.5">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" ht="15.5">
+      <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="15.5">
       <c r="A19" s="6"/>
     </row>
-    <row r="20" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="60">
       <c r="A20" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="30">
       <c r="B23" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="B24" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="B25" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="30">
       <c r="B26" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="30">
       <c r="A28" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="30">
+      <c r="B29" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="30">
+      <c r="B30" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="30">
+      <c r="B31" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="B32" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="7" t="s">
+    <row r="35" spans="1:2">
+      <c r="B35" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B30" s="7" t="s">
+    <row r="36" spans="1:2">
+      <c r="B36" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B31" s="7" t="s">
+    <row r="37" spans="1:2">
+      <c r="B37" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
+    <row r="39" spans="1:2">
+      <c r="A39" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" s="5" t="s">
+    <row r="40" spans="1:2">
+      <c r="B40" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
+    <row r="41" spans="1:2">
+      <c r="B41" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
+    <row r="42" spans="1:2">
+      <c r="B42" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
+    <row r="43" spans="1:2">
+      <c r="B43" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" ht="15.5">
       <c r="A45" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="202.8" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="202.75">
       <c r="A46" s="6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>